<commit_message>
rev 30/10 - ajustes gráficos
</commit_message>
<xml_diff>
--- a/modelo_indicadores/g12_comparativo_eqp_mes_combo.xlsx
+++ b/modelo_indicadores/g12_comparativo_eqp_mes_combo.xlsx
@@ -5,37 +5,25 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Downloads\modelo_indicadores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wopi.dropbox.com/wopi/files/oid_5573204658745166336/WOPIServiceId_TP_DROPBOX_PLUS/WOPIUserId_-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C22088-A400-4A23-A9C9-9C4A7EFA933D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{DCA7D1FF-EE40-441A-83DA-04626E152B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AE402F1-7D9D-4136-8C28-C538495CFFF4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Configurações" sheetId="1" r:id="rId1"/>
     <sheet name="Dados" sheetId="2" r:id="rId2"/>
     <sheet name="Cores" sheetId="3" r:id="rId3"/>
+    <sheet name="Eixos" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -55,37 +43,94 @@
     <t>Ordem</t>
   </si>
   <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>combo</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>1 coluna</t>
+  </si>
+  <si>
+    <t>ID_Gráfico</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Jan/2025</t>
+  </si>
+  <si>
+    <t>Fev/2025</t>
+  </si>
+  <si>
+    <t>Mar/2025</t>
+  </si>
+  <si>
+    <t>Abr/2025</t>
+  </si>
+  <si>
+    <t>Mai/2025</t>
+  </si>
+  <si>
+    <t>Jun/2025</t>
+  </si>
+  <si>
+    <t>Jul/2025</t>
+  </si>
+  <si>
+    <t>Ago/2025</t>
+  </si>
+  <si>
+    <t>Set/2025</t>
+  </si>
+  <si>
+    <t>Out/2025</t>
+  </si>
+  <si>
+    <t>Nov/2025</t>
+  </si>
+  <si>
+    <t>Dez/2025</t>
+  </si>
+  <si>
+    <t>Cor</t>
+  </si>
+  <si>
+    <t>Eixo Y</t>
+  </si>
+  <si>
+    <t>#d51d07</t>
+  </si>
+  <si>
     <t>bar</t>
   </si>
   <si>
-    <t>ID_Gráfico</t>
-  </si>
-  <si>
-    <t>Dataset</t>
-  </si>
-  <si>
-    <t>Cor</t>
-  </si>
-  <si>
-    <t>Rótulo</t>
-  </si>
-  <si>
-    <t>#d51d07</t>
+    <t>Esquerdo</t>
+  </si>
+  <si>
+    <t>#4284D7</t>
   </si>
   <si>
     <t>line</t>
   </si>
   <si>
-    <t>#4284D7</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>combo</t>
-  </si>
-  <si>
-    <t>2 coluna</t>
+    <t>Direito</t>
+  </si>
+  <si>
+    <t>Eixo</t>
+  </si>
+  <si>
+    <t>Mínimo</t>
+  </si>
+  <si>
+    <t>Máximo</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Comparativo de EQP Alocada</t>
@@ -101,9 +146,6 @@
   </si>
   <si>
     <t>EQP Real Acumulado</t>
-  </si>
-  <si>
-    <t>G12</t>
   </si>
 </sst>
 </file>
@@ -139,14 +181,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,9 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -523,25 +558,25 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:F1 A2 C2:F2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -550,164 +585,155 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.8984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.796875" customWidth="1"/>
+    <col min="2" max="2" width="20.796875" customWidth="1"/>
+    <col min="3" max="14" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="2">
-        <v>45658</v>
-      </c>
-      <c r="D1" s="2">
-        <v>45689</v>
-      </c>
-      <c r="E1" s="2">
-        <v>45717</v>
-      </c>
-      <c r="F1" s="2">
-        <v>45748</v>
-      </c>
-      <c r="G1" s="2">
-        <v>45778</v>
-      </c>
-      <c r="H1" s="2">
-        <v>45809</v>
-      </c>
-      <c r="I1" s="2">
-        <v>45839</v>
-      </c>
-      <c r="J1" s="2">
-        <v>45870</v>
-      </c>
-      <c r="K1" s="2">
-        <v>45901</v>
-      </c>
-      <c r="L1" s="2">
-        <v>45931</v>
-      </c>
-      <c r="M1" s="2">
-        <v>45962</v>
-      </c>
-      <c r="N1" s="2">
-        <v>45992</v>
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C2" s="1">
-        <v>62.006268997175411</v>
+        <v>62</v>
       </c>
       <c r="D2" s="1">
-        <v>68.566529144447799</v>
+        <v>69</v>
       </c>
       <c r="E2" s="1">
-        <v>79.133725058698175</v>
+        <v>79</v>
       </c>
       <c r="F2" s="1">
-        <v>304.86325164449363</v>
+        <v>305</v>
       </c>
       <c r="G2" s="1">
-        <v>457.00297691461219</v>
+        <v>457</v>
       </c>
       <c r="H2" s="1">
-        <v>635.82545615381559</v>
+        <v>636</v>
       </c>
       <c r="I2" s="1">
-        <v>896.6959994726725</v>
+        <v>897</v>
       </c>
       <c r="J2" s="1">
-        <v>980.42033627430521</v>
+        <v>980</v>
       </c>
       <c r="K2" s="1">
-        <v>1003.1101653329135</v>
+        <v>1003</v>
       </c>
       <c r="L2" s="1">
-        <v>991.04870487229857</v>
+        <v>991</v>
       </c>
       <c r="M2" s="1">
-        <v>931.656242644386</v>
+        <v>932</v>
       </c>
       <c r="N2" s="1">
-        <v>876.85568600775036</v>
+        <v>877</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1">
-        <v>62.006268997175411</v>
+        <v>62</v>
       </c>
       <c r="D3" s="1">
-        <v>130.5727981416232</v>
+        <v>131</v>
       </c>
       <c r="E3" s="1">
-        <v>209.70652320032139</v>
+        <v>210</v>
       </c>
       <c r="F3" s="1">
-        <v>514.56977484481502</v>
+        <v>515</v>
       </c>
       <c r="G3" s="1">
-        <v>971.57275175942721</v>
+        <v>972</v>
       </c>
       <c r="H3" s="1">
-        <v>1607.3982079132429</v>
+        <v>1607</v>
       </c>
       <c r="I3" s="1">
-        <v>2504.0942073859155</v>
+        <v>2504</v>
       </c>
       <c r="J3" s="1">
-        <v>3484.5145436602206</v>
+        <v>3485</v>
       </c>
       <c r="K3" s="1">
-        <v>4487.6247089931339</v>
+        <v>4488</v>
       </c>
       <c r="L3" s="1">
-        <v>5478.6734138654328</v>
+        <v>5479</v>
       </c>
       <c r="M3" s="1">
-        <v>6410.329656509819</v>
+        <v>6410</v>
       </c>
       <c r="N3" s="1">
-        <v>7287.1853425175696</v>
+        <v>7287</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1">
         <v>0</v>
@@ -748,10 +774,10 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
@@ -793,105 +819,191 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:B1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:N1 A5 A2 A3 A4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.796875" customWidth="1"/>
+    <col min="1" max="1" width="12.796875" customWidth="1"/>
+    <col min="2" max="3" width="20.796875" customWidth="1"/>
     <col min="4" max="4" width="15.796875" customWidth="1"/>
-    <col min="5" max="5" width="12.796875" customWidth="1"/>
+    <col min="5" max="6" width="12.796875" customWidth="1"/>
+    <col min="7" max="7" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
       </c>
       <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E1 C2:D2 D5 D4 D3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:F1 A5 A2 C2:F2 A3 C3:F3 A4 C4:F4 C5:F5" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="4" width="12.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:D3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>